<commit_message>
Replaced commas with full stops in size columns
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/MollEchino/Mol_raw/Mol_div_G2.xlsx
+++ b/Multi-taxa_data/MollEchino/Mol_raw/Mol_div_G2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\MollEchino\Mol_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85506E4-3E7A-484E-82DA-3ED46A87887D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEC9A8B-369E-41A9-AFA7-28895E37F7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="98">
   <si>
     <t>transect</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Prosobranchia</t>
   </si>
   <si>
-    <t>1,5</t>
-  </si>
-  <si>
     <t>Ginowan-RRD-12th-May-2022-15m-T1-P5120847</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Ginowan-RRD-12th-May-2022-15m-T1-P5120869</t>
   </si>
   <si>
-    <t>2,5</t>
-  </si>
-  <si>
     <t>Ginowan-RRD-12th-May-2022-15m-T1-P5120872</t>
   </si>
   <si>
@@ -192,9 +186,6 @@
   </si>
   <si>
     <t>JUE</t>
-  </si>
-  <si>
-    <t>3,5</t>
   </si>
   <si>
     <t>P5120482</t>
@@ -655,8 +646,8 @@
   </sheetPr>
   <dimension ref="A1:P999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -728,8 +719,8 @@
       <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>19</v>
+      <c r="K2" s="3">
+        <v>1.5</v>
       </c>
       <c r="M2" s="3"/>
     </row>
@@ -747,13 +738,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="3">
         <v>2</v>
@@ -774,13 +765,13 @@
         <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" s="3"/>
     </row>
@@ -798,16 +789,16 @@
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.5</v>
       </c>
       <c r="M5" s="3"/>
     </row>
@@ -825,16 +816,16 @@
         <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.5</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -852,13 +843,13 @@
         <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="M7" s="3"/>
     </row>
@@ -876,13 +867,13 @@
         <v>14</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M8" s="3"/>
     </row>
@@ -900,13 +891,13 @@
         <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K9" s="3">
         <v>1</v>
@@ -927,16 +918,16 @@
         <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -953,13 +944,13 @@
         <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -980,13 +971,13 @@
         <v>14</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K12" s="3">
         <v>2</v>
@@ -1010,13 +1001,13 @@
         <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1033,16 +1024,16 @@
         <v>14</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1059,13 +1050,13 @@
         <v>14</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K15" s="4">
         <v>1.5</v>
@@ -1085,7 +1076,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>16</v>
@@ -1094,7 +1085,7 @@
         <v>17</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="3">
         <v>4</v>
@@ -1114,16 +1105,16 @@
         <v>14</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K17" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1140,7 +1131,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>16</v>
@@ -1151,8 +1142,8 @@
       <c r="J18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>19</v>
+      <c r="K18" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1169,13 +1160,13 @@
         <v>14</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19" s="3">
         <v>2</v>
@@ -1195,16 +1186,16 @@
         <v>14</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K20" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1221,16 +1212,16 @@
         <v>14</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K21" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1247,16 +1238,16 @@
         <v>14</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K22" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1273,13 +1264,13 @@
         <v>14</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K23" s="3">
         <v>5</v>
@@ -1299,13 +1290,13 @@
         <v>14</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K24" s="3">
         <v>4</v>
@@ -1325,13 +1316,13 @@
         <v>14</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K25" s="3">
         <v>3</v>
@@ -1351,16 +1342,16 @@
         <v>14</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="K26" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1377,65 +1368,65 @@
         <v>14</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+      <c r="K28" s="3">
+        <v>3.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>17</v>
@@ -1446,28 +1437,28 @@
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K30" s="3">
         <v>5</v>
@@ -1475,7 +1466,7 @@
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>12</v>
@@ -1487,21 +1478,21 @@
         <v>14</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K31" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>12</v>
@@ -1513,13 +1504,13 @@
         <v>14</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K32" s="3">
         <v>5</v>
@@ -1527,7 +1518,7 @@
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>12</v>
@@ -1539,13 +1530,13 @@
         <v>14</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K33" s="3">
         <v>3</v>
@@ -1553,7 +1544,7 @@
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>12</v>
@@ -1565,13 +1556,13 @@
         <v>14</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K34" s="3">
         <v>3</v>
@@ -1579,7 +1570,7 @@
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>12</v>
@@ -1591,13 +1582,13 @@
         <v>14</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K35" s="3">
         <v>2</v>
@@ -1605,7 +1596,7 @@
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>12</v>
@@ -1617,21 +1608,21 @@
         <v>14</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K36" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>12</v>
@@ -1643,21 +1634,21 @@
         <v>14</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K37" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>12</v>
@@ -1669,13 +1660,13 @@
         <v>14</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K38" s="3">
         <v>2</v>
@@ -1683,7 +1674,7 @@
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>12</v>
@@ -1695,18 +1686,18 @@
         <v>14</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>12</v>
@@ -1718,13 +1709,13 @@
         <v>14</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K40" s="3">
         <v>3</v>
@@ -1732,7 +1723,7 @@
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>12</v>
@@ -1744,21 +1735,21 @@
         <v>14</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K41" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>12</v>
@@ -1770,47 +1761,47 @@
         <v>14</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K42" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="F43" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K43" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>12</v>
@@ -1822,13 +1813,13 @@
         <v>14</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K44" s="3">
         <v>3</v>
@@ -1836,7 +1827,7 @@
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>12</v>
@@ -1848,21 +1839,21 @@
         <v>14</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="K45" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>12</v>
@@ -1874,13 +1865,13 @@
         <v>14</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K46" s="3">
         <v>2</v>
@@ -1888,7 +1879,7 @@
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>12</v>
@@ -1900,13 +1891,13 @@
         <v>14</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K47" s="3">
         <v>2</v>
@@ -1914,7 +1905,7 @@
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -1926,13 +1917,13 @@
         <v>14</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K48" s="3">
         <v>2</v>
@@ -1940,7 +1931,7 @@
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>12</v>
@@ -1952,13 +1943,13 @@
         <v>14</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K49" s="3">
         <v>2</v>
@@ -1966,7 +1957,7 @@
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>12</v>
@@ -1978,21 +1969,21 @@
         <v>14</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K50" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>12</v>
@@ -2004,13 +1995,13 @@
         <v>14</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K51" s="3">
         <v>3</v>
@@ -2018,7 +2009,7 @@
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>12</v>
@@ -2030,13 +2021,13 @@
         <v>14</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K52" s="3">
         <v>4</v>
@@ -2044,7 +2035,7 @@
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>12</v>
@@ -2056,13 +2047,13 @@
         <v>14</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K53" s="3">
         <v>2</v>
@@ -2070,7 +2061,7 @@
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>12</v>
@@ -2082,13 +2073,13 @@
         <v>14</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K54" s="3">
         <v>2</v>
@@ -2096,54 +2087,54 @@
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="F55" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K55" s="3" t="s">
-        <v>19</v>
+      <c r="K55" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K56" s="3">
         <v>6</v>
@@ -2151,22 +2142,22 @@
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D57" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>17</v>
@@ -2177,28 +2168,28 @@
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D58" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K58" s="3">
         <v>2</v>
@@ -2206,22 +2197,22 @@
     </row>
     <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>17</v>
@@ -2233,51 +2224,51 @@
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K60" s="3" t="s">
-        <v>38</v>
+      <c r="K60" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="F61" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K61" s="3">
         <v>4</v>
@@ -2285,22 +2276,22 @@
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>17</v>
@@ -2311,22 +2302,22 @@
     </row>
     <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>17</v>
@@ -2337,22 +2328,22 @@
     </row>
     <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>17</v>
@@ -2363,48 +2354,48 @@
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K65" s="3" t="s">
-        <v>52</v>
+      <c r="K65" s="3">
+        <v>3.5</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>17</v>
@@ -2415,22 +2406,22 @@
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D67" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>17</v>
@@ -2441,28 +2432,28 @@
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D68" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J68" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K68" s="3">
         <v>1.5</v>
@@ -2470,25 +2461,25 @@
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K69" s="3">
         <v>7</v>
@@ -2496,28 +2487,28 @@
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K70" s="3">
         <v>3</v>
@@ -2525,28 +2516,28 @@
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="F71" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K71" s="3">
         <v>6</v>
@@ -2554,22 +2545,22 @@
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D72" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>17</v>

</xml_diff>